<commit_message>
- excel spreadsheet formatted
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\ULTERA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6EA592-51A5-438A-9BDE-71C0BF60CD3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD6410F-3608-4026-99F1-7A78FABFE39F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5334" yWindow="1572" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,220 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Name:</t>
   </si>
   <si>
     <t>Email:</t>
+  </si>
+  <si>
+    <t>Direct:</t>
+  </si>
+  <si>
+    <t>HandFetched:</t>
+  </si>
+  <si>
+    <t>Happy Researcher</t>
+  </si>
+  <si>
+    <t>happy@psu.edu</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>Material Comment</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Pointer</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe60 Ni20 Cr10 Zr10 </t>
+  </si>
+  <si>
+    <t>UTS</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Temperature [K]</t>
+  </si>
+  <si>
+    <t>Value [SI]</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>750*10^6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>10.1557/jmr.2018.153</t>
+  </si>
+  <si>
+    <t>BCC+FCC</t>
+  </si>
+  <si>
+    <t>QuickGuide</t>
+  </si>
+  <si>
+    <t>ElementFraction(space)…</t>
+  </si>
+  <si>
+    <t>HIP+A</t>
+  </si>
+  <si>
+    <t>optional information</t>
+  </si>
+  <si>
+    <t>ML/EXP/EM/DFT/THM</t>
+  </si>
+  <si>
+    <t>Absolute Temperature</t>
+  </si>
+  <si>
+    <t>Base SI Units s/Pa/m/kg</t>
+  </si>
+  <si>
+    <t>only DOI, no http etc</t>
+  </si>
+  <si>
+    <t>process1+process2  no space between</t>
+  </si>
+  <si>
+    <t>phase1+phase2        no space between</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>able</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>igure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ppendix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upplemental</t>
+    </r>
+  </si>
+  <si>
+    <t>id/nickname</t>
+  </si>
+  <si>
+    <t>Optional Upload Comments:</t>
+  </si>
+  <si>
+    <t>popular abbreviation or FullPropertyName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +246,106 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -62,14 +353,482 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,25 +1107,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.1015625" customWidth="1"/>
+    <col min="2" max="2" width="30.9453125" customWidth="1"/>
+    <col min="3" max="3" width="17.3671875" customWidth="1"/>
+    <col min="4" max="4" width="17.734375" customWidth="1"/>
+    <col min="5" max="6" width="17.7890625" customWidth="1"/>
+    <col min="7" max="7" width="18.62890625" customWidth="1"/>
+    <col min="8" max="8" width="18.5234375" customWidth="1"/>
+    <col min="9" max="9" width="19.68359375" customWidth="1"/>
+    <col min="10" max="10" width="17.7890625" customWidth="1"/>
+    <col min="11" max="11" width="32.5234375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="3" spans="1:11" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="10">
+        <v>298</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A8" s="2"/>
+      <c r="B8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="F2:K3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D357D88A-2775-40B2-B73F-2173296B7938}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Jupyter notebook uploader updates - Excel spreadsheet template updates
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\PycharmProjects\ULTERA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD6410F-3608-4026-99F1-7A78FABFE39F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61FEE11-3CCA-48CD-AE62-20ADAD65623B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Name:</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>none</t>
-  </si>
-  <si>
-    <t>750*10^6</t>
   </si>
   <si>
     <t>T7</t>
@@ -233,12 +230,42 @@
   <si>
     <t>popular abbreviation or FullPropertyName</t>
   </si>
+  <si>
+    <t>750e6</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>Col5</t>
+  </si>
+  <si>
+    <t>Scratch (NOT UPLOADED)</t>
+  </si>
+  <si>
+    <t>UTS in lb/in^2</t>
+  </si>
+  <si>
+    <t>Temperature in F</t>
+  </si>
+  <si>
+    <t>Some Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +333,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +377,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -695,6 +734,17 @@
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -702,128 +752,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1107,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1125,201 +1200,325 @@
     <col min="9" max="9" width="19.68359375" customWidth="1"/>
     <col min="10" max="10" width="17.7890625" customWidth="1"/>
     <col min="11" max="11" width="32.5234375" customWidth="1"/>
+    <col min="12" max="12" width="17.68359375" customWidth="1"/>
+    <col min="13" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="17.578125" customWidth="1"/>
+    <col min="16" max="16" width="17.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:16" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
+    </row>
+    <row r="3" spans="1:16" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+    </row>
+    <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="G5" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+    <row r="6" spans="1:16" ht="15.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
-    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>6</v>
+    <row r="7" spans="1:16" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="7">
+        <v>298</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="51" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="4" t="s">
+    <row r="8" spans="1:16" ht="20.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="43"/>
+      <c r="L8" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="50"/>
+    </row>
+    <row r="9" spans="1:16" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>38</v>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="P9" s="47" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
     </row>
-    <row r="7" spans="1:11" ht="15.9" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="10">
-        <v>298</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>29</v>
-      </c>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
     </row>
-    <row r="8" spans="1:11" ht="20.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A8" s="2"/>
-      <c r="B8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="20"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
     </row>
-    <row r="9" spans="1:11" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>19</v>
-      </c>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="K12" s="1"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="L8:P8"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="F2:K3"/>
@@ -1335,6 +1534,7 @@
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D357D88A-2775-40B2-B73F-2173296B7938}"/>
   </hyperlinks>

</xml_diff>